<commit_message>
Ajout des tableaux de bourses en FR et EN
</commit_message>
<xml_diff>
--- a/excel/locaux.xlsx
+++ b/excel/locaux.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD1EAA1-E1A4-704A-9044-11349CF96252}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED4B074-3A41-FE4B-80C8-10489A2636E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="560" windowWidth="16720" windowHeight="20380" xr2:uid="{FD29B0F2-1663-8540-80A1-3F866C889E60}"/>
   </bookViews>
@@ -521,7 +521,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
ajustement locaux et staff
</commit_message>
<xml_diff>
--- a/excel/locaux.xlsx
+++ b/excel/locaux.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D165112C-C542-AF46-80D4-6F10F4FFFA2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC7E4D4-FD4E-7B49-B494-B12E3781F91B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="68300" yWindow="560" windowWidth="34020" windowHeight="28180" xr2:uid="{FD29B0F2-1663-8540-80A1-3F866C889E60}"/>
+    <workbookView xWindow="34260" yWindow="500" windowWidth="34020" windowHeight="28180" activeTab="1" xr2:uid="{FD29B0F2-1663-8540-80A1-3F866C889E60}"/>
   </bookViews>
   <sheets>
     <sheet name="EQUIPES" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="60">
   <si>
     <t>Directeur technique</t>
   </si>
@@ -200,6 +200,21 @@
   </si>
   <si>
     <t>Awards ceremony&lt;br/&gt; Cegep de l'Abitibi-Témiscamingue</t>
+  </si>
+  <si>
+    <t>Sécurité Valcourt</t>
+  </si>
+  <si>
+    <t>Valcourt Securtiy services</t>
+  </si>
+  <si>
+    <t>Douches pour CO</t>
+  </si>
+  <si>
+    <t>0240&lt;br/&gt;0250</t>
+  </si>
+  <si>
+    <t>Volunteers showers</t>
   </si>
 </sst>
 </file>
@@ -610,7 +625,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72262817-9D66-6D48-97C4-5126E8F8BB18}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
@@ -829,8 +844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DDE1C1D-3050-7F46-8ECF-3B76DBA9970E}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1065,24 +1080,48 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="2"/>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B17" s="2"/>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="1">
+        <v>3110</v>
+      </c>
+      <c r="D16" s="1">
+        <f>C16</f>
+        <v>3110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="1" t="str">
+        <f>C17</f>
+        <v>0240&lt;br/&gt;0250</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="2"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="2"/>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" s="2"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="2"/>
     </row>
-    <row r="22" spans="2:3" ht="20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="20" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
       <c r="C22" s="10"/>
     </row>

</xml_diff>